<commit_message>
fixed BaseHistory stage clear
</commit_message>
<xml_diff>
--- a/JDE/JDE Table Master.xlsx
+++ b/JDE/JDE Table Master.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Business Reporting\ZDEV_BR_Sales\BRS\ETL\SSIS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Business Reporting\ZDEV\BR_Sales\BRS\JDE\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -12726,9 +12726,6 @@
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A3:L1996" totalsRowShown="0">
   <autoFilter ref="A3:L1996"/>
-  <sortState ref="A4:L1996">
-    <sortCondition ref="A3:A1996"/>
-  </sortState>
   <tableColumns count="12">
     <tableColumn id="1" name="TABLE_NAME"/>
     <tableColumn id="6" name="TABLE_TEXT"/>
@@ -14117,7 +14114,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E16" sqref="E16"/>
+      <selection pane="bottomLeft" activeCell="A985" sqref="A985"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="95.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
fix vendor reporting cube
</commit_message>
<xml_diff>
--- a/JDE/JDE Table Master.xlsx
+++ b/JDE/JDE Table Master.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17726"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Business Reporting\ZDEV\BR_Sales\BRS\JDE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Business Reporting\zDev\BR_Sales\BRS\JDE\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -22,7 +22,7 @@
     <definedName name="_xlnm.Print_Titles" localSheetId="2">'JDE Table Master'!$1:$3</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">Pricing!$1:$2</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
@@ -11306,7 +11306,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="3">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="[$-409]d\-mmm\-yy;@"/>
@@ -12726,6 +12726,9 @@
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A3:L1996" totalsRowShown="0">
   <autoFilter ref="A3:L1996"/>
+  <sortState ref="A4:L1996">
+    <sortCondition ref="A3:A1996"/>
+  </sortState>
   <tableColumns count="12">
     <tableColumn id="1" name="TABLE_NAME"/>
     <tableColumn id="6" name="TABLE_TEXT"/>
@@ -14113,8 +14116,8 @@
   <dimension ref="A1:L1996"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A985" sqref="A985"/>
+      <pane ySplit="3" topLeftCell="A1463" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B1472" sqref="B1472"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="95.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Add class & buygroup to supplier for vendor reporting
</commit_message>
<xml_diff>
--- a/JDE/JDE Table Master.xlsx
+++ b/JDE/JDE Table Master.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18201"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -14,12 +14,15 @@
   <sheets>
     <sheet name="Pricing" sheetId="3" r:id="rId1"/>
     <sheet name="ETL" sheetId="2" r:id="rId2"/>
-    <sheet name="JDE Table Master" sheetId="1" r:id="rId3"/>
+    <sheet name="US Shared" sheetId="5" r:id="rId3"/>
+    <sheet name="JDE Table Master" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">ETL!$A$3:$F$251</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'US Shared'!$A$1:$H$56</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="1">ETL!$1:$3</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="2">'JDE Table Master'!$1:$3</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="3">'JDE Table Master'!$1:$3</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">Pricing!$1:$2</definedName>
   </definedNames>
   <calcPr calcId="171027"/>
@@ -27,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13958" uniqueCount="3758">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14213" uniqueCount="3792">
   <si>
     <t>TABLE_NAME</t>
   </si>
@@ -11301,6 +11304,108 @@
   </si>
   <si>
     <t>zNO</t>
+  </si>
+  <si>
+    <t>Table</t>
+  </si>
+  <si>
+    <t>F0013</t>
+  </si>
+  <si>
+    <t>F55384</t>
+  </si>
+  <si>
+    <t>F55385</t>
+  </si>
+  <si>
+    <t>F55386</t>
+  </si>
+  <si>
+    <t>F554012</t>
+  </si>
+  <si>
+    <t>F5540122</t>
+  </si>
+  <si>
+    <t>F55512</t>
+  </si>
+  <si>
+    <t>F5602</t>
+  </si>
+  <si>
+    <t>F5604</t>
+  </si>
+  <si>
+    <t>F5611</t>
+  </si>
+  <si>
+    <t>F5614</t>
+  </si>
+  <si>
+    <t>F5640314</t>
+  </si>
+  <si>
+    <t>F5641</t>
+  </si>
+  <si>
+    <t>F564209</t>
+  </si>
+  <si>
+    <t>F5698</t>
+  </si>
+  <si>
+    <t>F5833</t>
+  </si>
+  <si>
+    <t>F5834</t>
+  </si>
+  <si>
+    <t>F5840122</t>
+  </si>
+  <si>
+    <t>F5840123</t>
+  </si>
+  <si>
+    <t>F5840124</t>
+  </si>
+  <si>
+    <t>F5865</t>
+  </si>
+  <si>
+    <t>F660102</t>
+  </si>
+  <si>
+    <t>F0150</t>
+  </si>
+  <si>
+    <t>LAST_ALTER</t>
+  </si>
+  <si>
+    <t>ED_TIMESTAMP</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>Bid - Reference - Supplier Items</t>
+  </si>
+  <si>
+    <t>ARCPDTA71</t>
+  </si>
+  <si>
+    <t>Bid - Reference - Descriptions</t>
+  </si>
+  <si>
+    <t>Bid - Reference - Item Extension</t>
+  </si>
+  <si>
+    <t>Pricing Sales Category by Major Product Class</t>
+  </si>
+  <si>
+    <t>DEA Registants File</t>
+  </si>
+  <si>
+    <t>Individual MB Contracts Pricing File</t>
   </si>
 </sst>
 </file>
@@ -11472,7 +11577,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -11655,6 +11760,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -11864,7 +11975,7 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
@@ -11903,6 +12014,10 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="5"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="47" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="46">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -13571,7 +13686,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C4" sqref="C4"/>
+      <selection pane="bottomLeft" activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14110,14 +14225,1375 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:H56"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="45.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" t="s">
+        <v>3782</v>
+      </c>
+      <c r="H1" t="s">
+        <v>3783</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>151</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2">
+        <v>18</v>
+      </c>
+      <c r="D2">
+        <v>109</v>
+      </c>
+      <c r="E2" t="s">
+        <v>152</v>
+      </c>
+      <c r="F2" t="s">
+        <v>3786</v>
+      </c>
+      <c r="G2" s="20">
+        <v>42625</v>
+      </c>
+      <c r="H2" s="23">
+        <v>0.55922918981481484</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>158</v>
+      </c>
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3">
+        <v>11</v>
+      </c>
+      <c r="D3">
+        <v>56</v>
+      </c>
+      <c r="E3" t="s">
+        <v>159</v>
+      </c>
+      <c r="F3" t="s">
+        <v>3786</v>
+      </c>
+      <c r="G3" s="20">
+        <v>42625</v>
+      </c>
+      <c r="H3" s="23">
+        <v>0.5544174652777778</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>347</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4">
+        <v>92</v>
+      </c>
+      <c r="D4">
+        <v>584</v>
+      </c>
+      <c r="E4" t="s">
+        <v>348</v>
+      </c>
+      <c r="F4" t="s">
+        <v>3786</v>
+      </c>
+      <c r="G4" s="20">
+        <v>42625</v>
+      </c>
+      <c r="H4" s="23">
+        <v>0.55922930555555561</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>413</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5">
+        <v>34</v>
+      </c>
+      <c r="D5">
+        <v>504</v>
+      </c>
+      <c r="E5" t="s">
+        <v>414</v>
+      </c>
+      <c r="F5" t="s">
+        <v>3786</v>
+      </c>
+      <c r="G5" s="20">
+        <v>42625</v>
+      </c>
+      <c r="H5" s="23">
+        <v>0.55922932870370368</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>441</v>
+      </c>
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6">
+        <v>14</v>
+      </c>
+      <c r="D6">
+        <v>128</v>
+      </c>
+      <c r="E6" t="s">
+        <v>442</v>
+      </c>
+      <c r="F6" t="s">
+        <v>3786</v>
+      </c>
+      <c r="G6" s="20">
+        <v>42625</v>
+      </c>
+      <c r="H6" s="23">
+        <v>0.55922934027777782</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>492</v>
+      </c>
+      <c r="B7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7">
+        <v>184</v>
+      </c>
+      <c r="D7">
+        <v>882</v>
+      </c>
+      <c r="E7" t="s">
+        <v>493</v>
+      </c>
+      <c r="F7" t="s">
+        <v>3786</v>
+      </c>
+      <c r="G7" s="20">
+        <v>42625</v>
+      </c>
+      <c r="H7" s="23">
+        <v>0.55922932870370368</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>553</v>
+      </c>
+      <c r="B8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8">
+        <v>101</v>
+      </c>
+      <c r="D8">
+        <v>516</v>
+      </c>
+      <c r="E8" t="s">
+        <v>554</v>
+      </c>
+      <c r="F8" t="s">
+        <v>3786</v>
+      </c>
+      <c r="G8" s="20">
+        <v>42625</v>
+      </c>
+      <c r="H8" s="23">
+        <v>0.55922934027777782</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>1654</v>
+      </c>
+      <c r="B9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9">
+        <v>37</v>
+      </c>
+      <c r="D9">
+        <v>154</v>
+      </c>
+      <c r="E9" t="s">
+        <v>1655</v>
+      </c>
+      <c r="F9" t="s">
+        <v>3786</v>
+      </c>
+      <c r="G9" s="20">
+        <v>42625</v>
+      </c>
+      <c r="H9" s="23">
+        <v>0.55585361111111109</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>1709</v>
+      </c>
+      <c r="B10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10">
+        <v>13</v>
+      </c>
+      <c r="D10">
+        <v>99</v>
+      </c>
+      <c r="E10" t="s">
+        <v>1710</v>
+      </c>
+      <c r="F10" t="s">
+        <v>3786</v>
+      </c>
+      <c r="G10" s="20">
+        <v>42625</v>
+      </c>
+      <c r="H10" s="23">
+        <v>0.55726989583333331</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>1715</v>
+      </c>
+      <c r="B11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11">
+        <v>35</v>
+      </c>
+      <c r="D11">
+        <v>308</v>
+      </c>
+      <c r="E11" t="s">
+        <v>1716</v>
+      </c>
+      <c r="F11" t="s">
+        <v>3786</v>
+      </c>
+      <c r="G11" s="20">
+        <v>42625</v>
+      </c>
+      <c r="H11" s="23">
+        <v>0.55726989583333331</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>1731</v>
+      </c>
+      <c r="B12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12">
+        <v>11</v>
+      </c>
+      <c r="D12">
+        <v>60</v>
+      </c>
+      <c r="E12" t="s">
+        <v>1732</v>
+      </c>
+      <c r="F12" t="s">
+        <v>3786</v>
+      </c>
+      <c r="G12" s="20">
+        <v>42625</v>
+      </c>
+      <c r="H12" s="23">
+        <v>0.55726994212962966</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>1749</v>
+      </c>
+      <c r="B13" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13">
+        <v>165</v>
+      </c>
+      <c r="D13">
+        <v>795</v>
+      </c>
+      <c r="E13" t="s">
+        <v>1750</v>
+      </c>
+      <c r="F13" t="s">
+        <v>3786</v>
+      </c>
+      <c r="G13" s="20">
+        <v>42625</v>
+      </c>
+      <c r="H13" s="23">
+        <v>0.55922890046296303</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>1774</v>
+      </c>
+      <c r="B14" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14">
+        <v>165</v>
+      </c>
+      <c r="D14">
+        <v>755</v>
+      </c>
+      <c r="E14" t="s">
+        <v>1775</v>
+      </c>
+      <c r="F14" t="s">
+        <v>3786</v>
+      </c>
+      <c r="G14" s="20">
+        <v>42625</v>
+      </c>
+      <c r="H14" s="23">
+        <v>0.55922876157407408</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>1798</v>
+      </c>
+      <c r="B15" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15">
+        <v>22</v>
+      </c>
+      <c r="D15">
+        <v>286</v>
+      </c>
+      <c r="E15" t="s">
+        <v>1799</v>
+      </c>
+      <c r="F15" t="s">
+        <v>3786</v>
+      </c>
+      <c r="G15" s="20">
+        <v>42625</v>
+      </c>
+      <c r="H15" s="23">
+        <v>0.55922875000000005</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>1800</v>
+      </c>
+      <c r="B16" t="s">
+        <v>12</v>
+      </c>
+      <c r="C16">
+        <v>21</v>
+      </c>
+      <c r="D16">
+        <v>214</v>
+      </c>
+      <c r="E16" t="s">
+        <v>1802</v>
+      </c>
+      <c r="F16" t="s">
+        <v>3786</v>
+      </c>
+      <c r="G16" s="20">
+        <v>42625</v>
+      </c>
+      <c r="H16" s="23">
+        <v>0.55922891203703706</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>2414</v>
+      </c>
+      <c r="B17" t="s">
+        <v>12</v>
+      </c>
+      <c r="C17">
+        <v>96</v>
+      </c>
+      <c r="D17">
+        <v>497</v>
+      </c>
+      <c r="E17" t="s">
+        <v>2415</v>
+      </c>
+      <c r="F17" t="s">
+        <v>3786</v>
+      </c>
+      <c r="G17" s="20">
+        <v>42625</v>
+      </c>
+      <c r="H17" s="23">
+        <v>0.55709123842592589</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>2416</v>
+      </c>
+      <c r="B18" t="s">
+        <v>12</v>
+      </c>
+      <c r="C18">
+        <v>60</v>
+      </c>
+      <c r="D18">
+        <v>329</v>
+      </c>
+      <c r="E18" t="s">
+        <v>2417</v>
+      </c>
+      <c r="F18" t="s">
+        <v>3786</v>
+      </c>
+      <c r="G18" s="20">
+        <v>42625</v>
+      </c>
+      <c r="H18" s="23">
+        <v>0.55922960648148146</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>3760</v>
+      </c>
+      <c r="B19" t="s">
+        <v>3784</v>
+      </c>
+      <c r="C19">
+        <v>29</v>
+      </c>
+      <c r="D19">
+        <v>708</v>
+      </c>
+      <c r="E19" t="s">
+        <v>3785</v>
+      </c>
+      <c r="F19" t="s">
+        <v>3786</v>
+      </c>
+      <c r="G19" s="20">
+        <v>42867</v>
+      </c>
+      <c r="H19" s="23">
+        <v>0.63624543981481485</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>3761</v>
+      </c>
+      <c r="B20" t="s">
+        <v>3784</v>
+      </c>
+      <c r="C20">
+        <v>9</v>
+      </c>
+      <c r="D20">
+        <v>445</v>
+      </c>
+      <c r="E20" t="s">
+        <v>3787</v>
+      </c>
+      <c r="F20" t="s">
+        <v>3786</v>
+      </c>
+      <c r="G20" s="20">
+        <v>42867</v>
+      </c>
+      <c r="H20" s="23">
+        <v>0.63624543981481485</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>3762</v>
+      </c>
+      <c r="B21" t="s">
+        <v>3784</v>
+      </c>
+      <c r="C21">
+        <v>12</v>
+      </c>
+      <c r="D21">
+        <v>464</v>
+      </c>
+      <c r="E21" t="s">
+        <v>3788</v>
+      </c>
+      <c r="F21" t="s">
+        <v>3786</v>
+      </c>
+      <c r="G21" s="20">
+        <v>42650</v>
+      </c>
+      <c r="H21" s="23">
+        <v>0.62406721064814819</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>2448</v>
+      </c>
+      <c r="B22" t="s">
+        <v>12</v>
+      </c>
+      <c r="C22">
+        <v>18</v>
+      </c>
+      <c r="D22">
+        <v>115</v>
+      </c>
+      <c r="E22" t="s">
+        <v>2449</v>
+      </c>
+      <c r="F22" t="s">
+        <v>3786</v>
+      </c>
+      <c r="G22" s="20">
+        <v>42625</v>
+      </c>
+      <c r="H22" s="23">
+        <v>0.55726989583333331</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>2473</v>
+      </c>
+      <c r="B23" t="s">
+        <v>12</v>
+      </c>
+      <c r="C23">
+        <v>40</v>
+      </c>
+      <c r="D23">
+        <v>243</v>
+      </c>
+      <c r="E23" t="s">
+        <v>2474</v>
+      </c>
+      <c r="F23" t="s">
+        <v>3786</v>
+      </c>
+      <c r="G23" s="20">
+        <v>42625</v>
+      </c>
+      <c r="H23" s="23">
+        <v>0.55922956018518521</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>2492</v>
+      </c>
+      <c r="B24" t="s">
+        <v>12</v>
+      </c>
+      <c r="C24">
+        <v>300</v>
+      </c>
+      <c r="D24">
+        <v>1757</v>
+      </c>
+      <c r="E24" t="s">
+        <v>2493</v>
+      </c>
+      <c r="F24" t="s">
+        <v>3786</v>
+      </c>
+      <c r="G24" s="20">
+        <v>42625</v>
+      </c>
+      <c r="H24" s="23">
+        <v>0.55922916666666667</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>2618</v>
+      </c>
+      <c r="B25" t="s">
+        <v>12</v>
+      </c>
+      <c r="C25">
+        <v>25</v>
+      </c>
+      <c r="D25">
+        <v>173</v>
+      </c>
+      <c r="E25" t="s">
+        <v>2619</v>
+      </c>
+      <c r="F25" t="s">
+        <v>3786</v>
+      </c>
+      <c r="G25" s="20">
+        <v>42625</v>
+      </c>
+      <c r="H25" s="23">
+        <v>0.55922890046296303</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>2642</v>
+      </c>
+      <c r="B26" t="s">
+        <v>12</v>
+      </c>
+      <c r="C26">
+        <v>39</v>
+      </c>
+      <c r="D26">
+        <v>362</v>
+      </c>
+      <c r="E26" t="s">
+        <v>2643</v>
+      </c>
+      <c r="F26" t="s">
+        <v>3786</v>
+      </c>
+      <c r="G26" s="20">
+        <v>42625</v>
+      </c>
+      <c r="H26" s="23">
+        <v>0.55922959490740742</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>2667</v>
+      </c>
+      <c r="B27" t="s">
+        <v>12</v>
+      </c>
+      <c r="C27">
+        <v>25</v>
+      </c>
+      <c r="D27">
+        <v>187</v>
+      </c>
+      <c r="E27" t="s">
+        <v>2668</v>
+      </c>
+      <c r="F27" t="s">
+        <v>3786</v>
+      </c>
+      <c r="G27" s="20">
+        <v>42625</v>
+      </c>
+      <c r="H27" s="23">
+        <v>0.55922890046296303</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>2702</v>
+      </c>
+      <c r="B28" t="s">
+        <v>12</v>
+      </c>
+      <c r="C28">
+        <v>231</v>
+      </c>
+      <c r="D28">
+        <v>3720</v>
+      </c>
+      <c r="F28" t="s">
+        <v>3786</v>
+      </c>
+      <c r="G28" s="20">
+        <v>42625</v>
+      </c>
+      <c r="H28" s="23">
+        <v>0.55922961805555549</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>2721</v>
+      </c>
+      <c r="B29" t="s">
+        <v>12</v>
+      </c>
+      <c r="C29">
+        <v>84</v>
+      </c>
+      <c r="D29">
+        <v>691</v>
+      </c>
+      <c r="E29" t="s">
+        <v>2722</v>
+      </c>
+      <c r="F29" t="s">
+        <v>3786</v>
+      </c>
+      <c r="G29" s="20">
+        <v>42628</v>
+      </c>
+      <c r="H29" s="23">
+        <v>0.59570064814814816</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>2725</v>
+      </c>
+      <c r="B30" t="s">
+        <v>12</v>
+      </c>
+      <c r="C30">
+        <v>51</v>
+      </c>
+      <c r="D30">
+        <v>374</v>
+      </c>
+      <c r="E30" t="s">
+        <v>2726</v>
+      </c>
+      <c r="F30" t="s">
+        <v>3786</v>
+      </c>
+      <c r="G30" s="20">
+        <v>42625</v>
+      </c>
+      <c r="H30" s="23">
+        <v>0.55756822916666671</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>2727</v>
+      </c>
+      <c r="B31" t="s">
+        <v>12</v>
+      </c>
+      <c r="C31">
+        <v>42</v>
+      </c>
+      <c r="D31">
+        <v>267</v>
+      </c>
+      <c r="E31" t="s">
+        <v>2728</v>
+      </c>
+      <c r="F31" t="s">
+        <v>3786</v>
+      </c>
+      <c r="G31" s="20">
+        <v>42625</v>
+      </c>
+      <c r="H31" s="23">
+        <v>0.55756824074074074</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>2729</v>
+      </c>
+      <c r="B32" t="s">
+        <v>12</v>
+      </c>
+      <c r="C32">
+        <v>12</v>
+      </c>
+      <c r="D32">
+        <v>101</v>
+      </c>
+      <c r="E32" t="s">
+        <v>2730</v>
+      </c>
+      <c r="F32" t="s">
+        <v>3786</v>
+      </c>
+      <c r="G32" s="20">
+        <v>42625</v>
+      </c>
+      <c r="H32" s="23">
+        <v>0.55756821759259256</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>3763</v>
+      </c>
+      <c r="B33" t="s">
+        <v>12</v>
+      </c>
+      <c r="C33">
+        <v>18</v>
+      </c>
+      <c r="D33">
+        <v>98</v>
+      </c>
+      <c r="E33" t="s">
+        <v>3789</v>
+      </c>
+      <c r="F33" t="s">
+        <v>3786</v>
+      </c>
+      <c r="G33" s="20">
+        <v>42108</v>
+      </c>
+      <c r="H33" s="23">
+        <v>0.64862504629629625</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>3769</v>
+      </c>
+      <c r="B34" t="s">
+        <v>12</v>
+      </c>
+      <c r="C34">
+        <v>19</v>
+      </c>
+      <c r="D34">
+        <v>238</v>
+      </c>
+      <c r="E34" t="s">
+        <v>3790</v>
+      </c>
+      <c r="F34" t="s">
+        <v>3786</v>
+      </c>
+      <c r="G34" s="20">
+        <v>41939</v>
+      </c>
+      <c r="H34" s="23">
+        <v>0.86599032407407417</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>3778</v>
+      </c>
+      <c r="B35" t="s">
+        <v>12</v>
+      </c>
+      <c r="C35">
+        <v>16</v>
+      </c>
+      <c r="D35">
+        <v>115</v>
+      </c>
+      <c r="E35" t="s">
+        <v>3791</v>
+      </c>
+      <c r="F35" t="s">
+        <v>3786</v>
+      </c>
+      <c r="G35" s="20">
+        <v>41740</v>
+      </c>
+      <c r="H35" s="23">
+        <v>0.62420861111111114</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>3776</v>
+      </c>
+      <c r="B36" t="s">
+        <v>12</v>
+      </c>
+      <c r="C36">
+        <v>20</v>
+      </c>
+      <c r="D36">
+        <v>119</v>
+      </c>
+      <c r="F36" t="s">
+        <v>3786</v>
+      </c>
+      <c r="G36" s="20">
+        <v>41413</v>
+      </c>
+      <c r="H36" s="23">
+        <v>8.7360601851851849E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>3777</v>
+      </c>
+      <c r="B37" t="s">
+        <v>12</v>
+      </c>
+      <c r="C37">
+        <v>12</v>
+      </c>
+      <c r="D37">
+        <v>90</v>
+      </c>
+      <c r="F37" t="s">
+        <v>3786</v>
+      </c>
+      <c r="G37" s="20">
+        <v>41413</v>
+      </c>
+      <c r="H37" s="23">
+        <v>8.7362951388888888E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>3779</v>
+      </c>
+      <c r="B38" t="s">
+        <v>12</v>
+      </c>
+      <c r="C38">
+        <v>25</v>
+      </c>
+      <c r="D38">
+        <v>411</v>
+      </c>
+      <c r="F38" t="s">
+        <v>3786</v>
+      </c>
+      <c r="G38" s="20">
+        <v>41410</v>
+      </c>
+      <c r="H38" s="23">
+        <v>0.50206951388888887</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>3770</v>
+      </c>
+      <c r="B39" t="s">
+        <v>12</v>
+      </c>
+      <c r="C39">
+        <v>17</v>
+      </c>
+      <c r="D39">
+        <v>118</v>
+      </c>
+      <c r="F39" t="s">
+        <v>3786</v>
+      </c>
+      <c r="G39" s="20">
+        <v>41017</v>
+      </c>
+      <c r="H39" s="23">
+        <v>4.7388194444444439E-3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>3764</v>
+      </c>
+      <c r="B40" t="s">
+        <v>12</v>
+      </c>
+      <c r="C40">
+        <v>19</v>
+      </c>
+      <c r="D40">
+        <v>114</v>
+      </c>
+      <c r="F40" t="s">
+        <v>3786</v>
+      </c>
+      <c r="G40" s="20">
+        <v>41006</v>
+      </c>
+      <c r="H40" s="23">
+        <v>0.15572981481481482</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>3644</v>
+      </c>
+      <c r="B41" t="s">
+        <v>12</v>
+      </c>
+      <c r="C41">
+        <v>23</v>
+      </c>
+      <c r="D41">
+        <v>193</v>
+      </c>
+      <c r="F41" t="s">
+        <v>3786</v>
+      </c>
+      <c r="G41" s="20">
+        <v>40515</v>
+      </c>
+      <c r="H41" s="23">
+        <v>0.37460487268518516</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>3766</v>
+      </c>
+      <c r="B42" t="s">
+        <v>12</v>
+      </c>
+      <c r="C42">
+        <v>41</v>
+      </c>
+      <c r="D42">
+        <v>276</v>
+      </c>
+      <c r="F42" t="s">
+        <v>3786</v>
+      </c>
+      <c r="G42" s="20">
+        <v>39487</v>
+      </c>
+      <c r="H42" s="23">
+        <v>0.25032361111111112</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>3781</v>
+      </c>
+      <c r="B43" t="s">
+        <v>12</v>
+      </c>
+      <c r="C43">
+        <v>12</v>
+      </c>
+      <c r="D43">
+        <v>110</v>
+      </c>
+      <c r="F43" t="s">
+        <v>3786</v>
+      </c>
+      <c r="G43" s="20">
+        <v>39486</v>
+      </c>
+      <c r="H43" s="23">
+        <v>0.39357087962962961</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>3645</v>
+      </c>
+      <c r="B44" t="s">
+        <v>12</v>
+      </c>
+      <c r="C44">
+        <v>9</v>
+      </c>
+      <c r="D44">
+        <v>637</v>
+      </c>
+      <c r="F44" t="s">
+        <v>3786</v>
+      </c>
+      <c r="G44" s="20">
+        <v>39486</v>
+      </c>
+      <c r="H44" s="23">
+        <v>0.21075917824074075</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>3767</v>
+      </c>
+      <c r="B45" t="s">
+        <v>12</v>
+      </c>
+      <c r="C45">
+        <v>30</v>
+      </c>
+      <c r="D45">
+        <v>293</v>
+      </c>
+      <c r="F45" t="s">
+        <v>3786</v>
+      </c>
+      <c r="G45" s="20">
+        <v>39486</v>
+      </c>
+      <c r="H45" s="23">
+        <v>0.29502784722222225</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>3768</v>
+      </c>
+      <c r="B46" t="s">
+        <v>12</v>
+      </c>
+      <c r="C46">
+        <v>14</v>
+      </c>
+      <c r="D46">
+        <v>92</v>
+      </c>
+      <c r="F46" t="s">
+        <v>3786</v>
+      </c>
+      <c r="G46" s="20">
+        <v>39486</v>
+      </c>
+      <c r="H46" s="23">
+        <v>0.2950538425925926</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>3765</v>
+      </c>
+      <c r="B47" t="s">
+        <v>12</v>
+      </c>
+      <c r="C47">
+        <v>8</v>
+      </c>
+      <c r="D47">
+        <v>52</v>
+      </c>
+      <c r="F47" t="s">
+        <v>3786</v>
+      </c>
+      <c r="G47" s="20">
+        <v>39478</v>
+      </c>
+      <c r="H47" s="23">
+        <v>0.6515180439814815</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>3773</v>
+      </c>
+      <c r="B48" t="s">
+        <v>12</v>
+      </c>
+      <c r="C48">
+        <v>37</v>
+      </c>
+      <c r="D48">
+        <v>333</v>
+      </c>
+      <c r="F48" t="s">
+        <v>3786</v>
+      </c>
+      <c r="G48" s="20">
+        <v>39465</v>
+      </c>
+      <c r="H48" s="23">
+        <v>0.51796172453703704</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>3771</v>
+      </c>
+      <c r="B49" t="s">
+        <v>12</v>
+      </c>
+      <c r="C49">
+        <v>11</v>
+      </c>
+      <c r="D49">
+        <v>135</v>
+      </c>
+      <c r="F49" t="s">
+        <v>3786</v>
+      </c>
+      <c r="G49" s="20">
+        <v>39370</v>
+      </c>
+      <c r="H49" s="23">
+        <v>0.49657274305555554</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>3772</v>
+      </c>
+      <c r="B50" t="s">
+        <v>12</v>
+      </c>
+      <c r="C50">
+        <v>37</v>
+      </c>
+      <c r="D50">
+        <v>282</v>
+      </c>
+      <c r="F50" t="s">
+        <v>3786</v>
+      </c>
+      <c r="G50" s="20">
+        <v>39303</v>
+      </c>
+      <c r="H50" s="23">
+        <v>0.74039734953703695</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>3759</v>
+      </c>
+      <c r="B51" t="s">
+        <v>12</v>
+      </c>
+      <c r="C51">
+        <v>10</v>
+      </c>
+      <c r="D51">
+        <v>87</v>
+      </c>
+      <c r="F51" t="s">
+        <v>3786</v>
+      </c>
+      <c r="G51" s="20">
+        <v>39121</v>
+      </c>
+      <c r="H51" s="23">
+        <v>0.42892013888888886</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>3774</v>
+      </c>
+      <c r="B52" t="s">
+        <v>12</v>
+      </c>
+      <c r="C52">
+        <v>92</v>
+      </c>
+      <c r="D52">
+        <v>675</v>
+      </c>
+      <c r="F52" t="s">
+        <v>3786</v>
+      </c>
+      <c r="G52" s="20">
+        <v>39072</v>
+      </c>
+      <c r="H52" s="23">
+        <v>0.45860575231481482</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>3775</v>
+      </c>
+      <c r="B53" t="s">
+        <v>12</v>
+      </c>
+      <c r="C53">
+        <v>53</v>
+      </c>
+      <c r="D53">
+        <v>355</v>
+      </c>
+      <c r="F53" t="s">
+        <v>3786</v>
+      </c>
+      <c r="G53" s="20">
+        <v>39072</v>
+      </c>
+      <c r="H53" s="23">
+        <v>0.45864018518518518</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="55" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="56" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <autoFilter ref="A1:H56">
+    <filterColumn colId="6">
+      <filters>
+        <dateGroupItem year="2017" dateTimeGrouping="year"/>
+        <dateGroupItem year="2016" dateTimeGrouping="year"/>
+      </filters>
+    </filterColumn>
+    <sortState ref="A2:H32">
+      <sortCondition ref="A1:A56"/>
+    </sortState>
+  </autoFilter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:L1996"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A1463" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B1472" sqref="B1472"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="95.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -85112,4 +86588,536 @@
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C55"/>
+  <sheetViews>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A55"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="8" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="21" t="s">
+        <v>3758</v>
+      </c>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="21" t="s">
+        <v>3759</v>
+      </c>
+      <c r="B2" s="21" t="e">
+        <f>+VLOOKUP(A2,'JDE Table Master'!$A:$A,1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="C2" s="21"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="21" t="s">
+        <v>151</v>
+      </c>
+      <c r="B3" s="21" t="str">
+        <f>+VLOOKUP(A3,'JDE Table Master'!$A:$A,1,0)</f>
+        <v>F0014</v>
+      </c>
+      <c r="C3" s="21"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="21" t="s">
+        <v>158</v>
+      </c>
+      <c r="B4" s="21" t="str">
+        <f>+VLOOKUP(A4,'JDE Table Master'!$A:$A,1,0)</f>
+        <v>F0015</v>
+      </c>
+      <c r="C4" s="21"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="21" t="s">
+        <v>413</v>
+      </c>
+      <c r="B5" s="21" t="str">
+        <f>+VLOOKUP(A5,'JDE Table Master'!$A:$A,1,0)</f>
+        <v>F0111</v>
+      </c>
+      <c r="C5" s="21"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="21" t="s">
+        <v>441</v>
+      </c>
+      <c r="B6" s="21" t="str">
+        <f>+VLOOKUP(A6,'JDE Table Master'!$A:$A,1,0)</f>
+        <v>F0115</v>
+      </c>
+      <c r="C6" s="21"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="21" t="s">
+        <v>492</v>
+      </c>
+      <c r="B7" s="21" t="str">
+        <f>+VLOOKUP(A7,'JDE Table Master'!$A:$A,1,0)</f>
+        <v>F0301</v>
+      </c>
+      <c r="C7" s="21"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="21" t="s">
+        <v>553</v>
+      </c>
+      <c r="B8" s="21" t="str">
+        <f>+VLOOKUP(A8,'JDE Table Master'!$A:$A,1,0)</f>
+        <v>F0401</v>
+      </c>
+      <c r="C8" s="21"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="21" t="s">
+        <v>1654</v>
+      </c>
+      <c r="B9" s="21" t="str">
+        <f>+VLOOKUP(A9,'JDE Table Master'!$A:$A,1,0)</f>
+        <v>F40205</v>
+      </c>
+      <c r="C9" s="21" t="s">
+        <v>1668</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="21" t="s">
+        <v>1774</v>
+      </c>
+      <c r="B10" s="21" t="str">
+        <f>+VLOOKUP(A10,'JDE Table Master'!$A:$A,1,0)</f>
+        <v>F4102</v>
+      </c>
+      <c r="C10" s="21" t="s">
+        <v>3651</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="21" t="s">
+        <v>1798</v>
+      </c>
+      <c r="B11" s="21" t="str">
+        <f>+VLOOKUP(A11,'JDE Table Master'!$A:$A,1,0)</f>
+        <v>F4104</v>
+      </c>
+      <c r="C11" s="21" t="s">
+        <v>3648</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="21" t="s">
+        <v>1800</v>
+      </c>
+      <c r="B12" s="21" t="str">
+        <f>+VLOOKUP(A12,'JDE Table Master'!$A:$A,1,0)</f>
+        <v>F4105</v>
+      </c>
+      <c r="C12" s="21"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="21" t="s">
+        <v>2414</v>
+      </c>
+      <c r="B13" s="21" t="str">
+        <f>+VLOOKUP(A13,'JDE Table Master'!$A:$A,1,0)</f>
+        <v>F5501</v>
+      </c>
+      <c r="C13" s="21"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="21" t="s">
+        <v>2416</v>
+      </c>
+      <c r="B14" s="21" t="str">
+        <f>+VLOOKUP(A14,'JDE Table Master'!$A:$A,1,0)</f>
+        <v>F550101</v>
+      </c>
+      <c r="C14" s="21"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="21" t="s">
+        <v>3645</v>
+      </c>
+      <c r="B15" s="21" t="e">
+        <f>+VLOOKUP(A15,'JDE Table Master'!$A:$A,1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="C15" s="21"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="21" t="s">
+        <v>3760</v>
+      </c>
+      <c r="B16" s="21" t="e">
+        <f>+VLOOKUP(A16,'JDE Table Master'!$A:$A,1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="C16" s="21"/>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="21" t="s">
+        <v>3761</v>
+      </c>
+      <c r="B17" s="21" t="e">
+        <f>+VLOOKUP(A17,'JDE Table Master'!$A:$A,1,0)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="21" t="s">
+        <v>3762</v>
+      </c>
+      <c r="B18" s="21" t="e">
+        <f>+VLOOKUP(A18,'JDE Table Master'!$A:$A,1,0)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="21" t="s">
+        <v>3763</v>
+      </c>
+      <c r="B19" s="21" t="e">
+        <f>+VLOOKUP(A19,'JDE Table Master'!$A:$A,1,0)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="21" t="s">
+        <v>3764</v>
+      </c>
+      <c r="B20" s="21" t="e">
+        <f>+VLOOKUP(A20,'JDE Table Master'!$A:$A,1,0)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="21" t="s">
+        <v>2448</v>
+      </c>
+      <c r="B21" s="21" t="str">
+        <f>+VLOOKUP(A21,'JDE Table Master'!$A:$A,1,0)</f>
+        <v>F554070</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="21" t="s">
+        <v>2473</v>
+      </c>
+      <c r="B22" s="21" t="str">
+        <f>+VLOOKUP(A22,'JDE Table Master'!$A:$A,1,0)</f>
+        <v>F55510</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="21" t="s">
+        <v>3765</v>
+      </c>
+      <c r="B23" s="21" t="e">
+        <f>+VLOOKUP(A23,'JDE Table Master'!$A:$A,1,0)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="21" t="s">
+        <v>2492</v>
+      </c>
+      <c r="B24" s="21" t="str">
+        <f>+VLOOKUP(A24,'JDE Table Master'!$A:$A,1,0)</f>
+        <v>F55520</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="21" t="s">
+        <v>3766</v>
+      </c>
+      <c r="B25" s="21" t="e">
+        <f>+VLOOKUP(A25,'JDE Table Master'!$A:$A,1,0)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="21" t="s">
+        <v>3767</v>
+      </c>
+      <c r="B26" s="21" t="e">
+        <f>+VLOOKUP(A26,'JDE Table Master'!$A:$A,1,0)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="21" t="s">
+        <v>3768</v>
+      </c>
+      <c r="B27" s="21" t="e">
+        <f>+VLOOKUP(A27,'JDE Table Master'!$A:$A,1,0)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="21" t="s">
+        <v>3769</v>
+      </c>
+      <c r="B28" s="21" t="e">
+        <f>+VLOOKUP(A28,'JDE Table Master'!$A:$A,1,0)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="21" t="s">
+        <v>3770</v>
+      </c>
+      <c r="B29" s="21" t="e">
+        <f>+VLOOKUP(A29,'JDE Table Master'!$A:$A,1,0)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="21" t="s">
+        <v>3771</v>
+      </c>
+      <c r="B30" s="21" t="e">
+        <f>+VLOOKUP(A30,'JDE Table Master'!$A:$A,1,0)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="21" t="s">
+        <v>2642</v>
+      </c>
+      <c r="B31" s="21" t="str">
+        <f>+VLOOKUP(A31,'JDE Table Master'!$A:$A,1,0)</f>
+        <v>F56416</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="21" t="s">
+        <v>3772</v>
+      </c>
+      <c r="B32" s="21" t="e">
+        <f>+VLOOKUP(A32,'JDE Table Master'!$A:$A,1,0)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="21" t="s">
+        <v>2702</v>
+      </c>
+      <c r="B33" s="21" t="str">
+        <f>+VLOOKUP(A33,'JDE Table Master'!$A:$A,1,0)</f>
+        <v>F56961</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="21" t="s">
+        <v>3773</v>
+      </c>
+      <c r="B34" s="21" t="e">
+        <f>+VLOOKUP(A34,'JDE Table Master'!$A:$A,1,0)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="21" t="s">
+        <v>2721</v>
+      </c>
+      <c r="B35" s="21" t="str">
+        <f>+VLOOKUP(A35,'JDE Table Master'!$A:$A,1,0)</f>
+        <v>F5830</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="21" t="s">
+        <v>2725</v>
+      </c>
+      <c r="B36" s="21" t="str">
+        <f>+VLOOKUP(A36,'JDE Table Master'!$A:$A,1,0)</f>
+        <v>F5831</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="21" t="s">
+        <v>2727</v>
+      </c>
+      <c r="B37" s="21" t="str">
+        <f>+VLOOKUP(A37,'JDE Table Master'!$A:$A,1,0)</f>
+        <v>F5832</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="21" t="s">
+        <v>3774</v>
+      </c>
+      <c r="B38" s="21" t="e">
+        <f>+VLOOKUP(A38,'JDE Table Master'!$A:$A,1,0)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="21" t="s">
+        <v>3775</v>
+      </c>
+      <c r="B39" s="21" t="e">
+        <f>+VLOOKUP(A39,'JDE Table Master'!$A:$A,1,0)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="21" t="s">
+        <v>3776</v>
+      </c>
+      <c r="B40" s="21" t="e">
+        <f>+VLOOKUP(A40,'JDE Table Master'!$A:$A,1,0)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="21" t="s">
+        <v>3777</v>
+      </c>
+      <c r="B41" s="21" t="e">
+        <f>+VLOOKUP(A41,'JDE Table Master'!$A:$A,1,0)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" s="21" t="s">
+        <v>3778</v>
+      </c>
+      <c r="B42" s="21" t="e">
+        <f>+VLOOKUP(A42,'JDE Table Master'!$A:$A,1,0)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" s="21" t="s">
+        <v>2729</v>
+      </c>
+      <c r="B43" s="21" t="str">
+        <f>+VLOOKUP(A43,'JDE Table Master'!$A:$A,1,0)</f>
+        <v>F5844</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" s="21" t="s">
+        <v>3779</v>
+      </c>
+      <c r="B44" s="21" t="e">
+        <f>+VLOOKUP(A44,'JDE Table Master'!$A:$A,1,0)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" s="21" t="s">
+        <v>3780</v>
+      </c>
+      <c r="B45" s="21" t="e">
+        <f>+VLOOKUP(A45,'JDE Table Master'!$A:$A,1,0)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" s="22" t="s">
+        <v>3649</v>
+      </c>
+      <c r="B46" s="21" t="e">
+        <f>+VLOOKUP(A46,'JDE Table Master'!$A:$A,1,0)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" s="22" t="s">
+        <v>347</v>
+      </c>
+      <c r="B47" s="21" t="str">
+        <f>+VLOOKUP(A47,'JDE Table Master'!$A:$A,1,0)</f>
+        <v>F0101</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" s="22" t="s">
+        <v>3781</v>
+      </c>
+      <c r="B48" s="21" t="e">
+        <f>+VLOOKUP(A48,'JDE Table Master'!$A:$A,1,0)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" s="22" t="s">
+        <v>1709</v>
+      </c>
+      <c r="B49" s="21" t="str">
+        <f>+VLOOKUP(A49,'JDE Table Master'!$A:$A,1,0)</f>
+        <v>F4070</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" s="22" t="s">
+        <v>1715</v>
+      </c>
+      <c r="B50" s="21" t="str">
+        <f>+VLOOKUP(A50,'JDE Table Master'!$A:$A,1,0)</f>
+        <v>F4072</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" s="22" t="s">
+        <v>1731</v>
+      </c>
+      <c r="B51" s="21" t="str">
+        <f>+VLOOKUP(A51,'JDE Table Master'!$A:$A,1,0)</f>
+        <v>F4094</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" s="22" t="s">
+        <v>1749</v>
+      </c>
+      <c r="B52" s="21" t="str">
+        <f>+VLOOKUP(A52,'JDE Table Master'!$A:$A,1,0)</f>
+        <v>F4101</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" s="22" t="s">
+        <v>3644</v>
+      </c>
+      <c r="B53" s="21" t="e">
+        <f>+VLOOKUP(A53,'JDE Table Master'!$A:$A,1,0)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" s="22" t="s">
+        <v>2618</v>
+      </c>
+      <c r="B54" s="21" t="str">
+        <f>+VLOOKUP(A54,'JDE Table Master'!$A:$A,1,0)</f>
+        <v>F5613</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" s="22" t="s">
+        <v>2667</v>
+      </c>
+      <c r="B55" s="21" t="str">
+        <f>+VLOOKUP(A55,'JDE Table Master'!$A:$A,1,0)</f>
+        <v>F5656</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
automate DS batach load using SQLCMD
</commit_message>
<xml_diff>
--- a/JDE/JDE Table Master.xlsx
+++ b/JDE/JDE Table Master.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13935" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13935" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Pricing" sheetId="3" r:id="rId1"/>
@@ -14225,11 +14225,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1"/>
-  <dimension ref="A1:H56"/>
+  <dimension ref="A1:H53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="A8" sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14272,45 +14271,42 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>151</v>
+        <v>3759</v>
       </c>
       <c r="B2" t="s">
         <v>12</v>
       </c>
       <c r="C2">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="D2">
-        <v>109</v>
-      </c>
-      <c r="E2" t="s">
-        <v>152</v>
+        <v>87</v>
       </c>
       <c r="F2" t="s">
         <v>3786</v>
       </c>
       <c r="G2" s="20">
-        <v>42625</v>
+        <v>39121</v>
       </c>
       <c r="H2" s="23">
-        <v>0.55922918981481484</v>
+        <v>0.42892013888888886</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="B3" t="s">
         <v>12</v>
       </c>
       <c r="C3">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="D3">
-        <v>56</v>
+        <v>109</v>
       </c>
       <c r="E3" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="F3" t="s">
         <v>3786</v>
@@ -14319,24 +14315,24 @@
         <v>42625</v>
       </c>
       <c r="H3" s="23">
-        <v>0.5544174652777778</v>
+        <v>0.55922918981481484</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>347</v>
+        <v>158</v>
       </c>
       <c r="B4" t="s">
         <v>12</v>
       </c>
       <c r="C4">
-        <v>92</v>
+        <v>11</v>
       </c>
       <c r="D4">
-        <v>584</v>
+        <v>56</v>
       </c>
       <c r="E4" t="s">
-        <v>348</v>
+        <v>159</v>
       </c>
       <c r="F4" t="s">
         <v>3786</v>
@@ -14345,24 +14341,24 @@
         <v>42625</v>
       </c>
       <c r="H4" s="23">
-        <v>0.55922930555555561</v>
+        <v>0.5544174652777778</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>413</v>
+        <v>347</v>
       </c>
       <c r="B5" t="s">
         <v>12</v>
       </c>
       <c r="C5">
-        <v>34</v>
+        <v>92</v>
       </c>
       <c r="D5">
-        <v>504</v>
+        <v>584</v>
       </c>
       <c r="E5" t="s">
-        <v>414</v>
+        <v>348</v>
       </c>
       <c r="F5" t="s">
         <v>3786</v>
@@ -14371,24 +14367,24 @@
         <v>42625</v>
       </c>
       <c r="H5" s="23">
-        <v>0.55922932870370368</v>
+        <v>0.55922930555555561</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>441</v>
+        <v>413</v>
       </c>
       <c r="B6" t="s">
         <v>12</v>
       </c>
       <c r="C6">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="D6">
-        <v>128</v>
+        <v>504</v>
       </c>
       <c r="E6" t="s">
-        <v>442</v>
+        <v>414</v>
       </c>
       <c r="F6" t="s">
         <v>3786</v>
@@ -14397,24 +14393,24 @@
         <v>42625</v>
       </c>
       <c r="H6" s="23">
-        <v>0.55922934027777782</v>
+        <v>0.55922932870370368</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>492</v>
+        <v>441</v>
       </c>
       <c r="B7" t="s">
         <v>12</v>
       </c>
       <c r="C7">
-        <v>184</v>
+        <v>14</v>
       </c>
       <c r="D7">
-        <v>882</v>
+        <v>128</v>
       </c>
       <c r="E7" t="s">
-        <v>493</v>
+        <v>442</v>
       </c>
       <c r="F7" t="s">
         <v>3786</v>
@@ -14423,50 +14419,47 @@
         <v>42625</v>
       </c>
       <c r="H7" s="23">
-        <v>0.55922932870370368</v>
+        <v>0.55922934027777782</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>553</v>
+        <v>3781</v>
       </c>
       <c r="B8" t="s">
         <v>12</v>
       </c>
       <c r="C8">
-        <v>101</v>
+        <v>12</v>
       </c>
       <c r="D8">
-        <v>516</v>
-      </c>
-      <c r="E8" t="s">
-        <v>554</v>
+        <v>110</v>
       </c>
       <c r="F8" t="s">
         <v>3786</v>
       </c>
       <c r="G8" s="20">
-        <v>42625</v>
+        <v>39486</v>
       </c>
       <c r="H8" s="23">
-        <v>0.55922934027777782</v>
+        <v>0.39357087962962961</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>1654</v>
+        <v>492</v>
       </c>
       <c r="B9" t="s">
         <v>12</v>
       </c>
       <c r="C9">
-        <v>37</v>
+        <v>184</v>
       </c>
       <c r="D9">
-        <v>154</v>
+        <v>882</v>
       </c>
       <c r="E9" t="s">
-        <v>1655</v>
+        <v>493</v>
       </c>
       <c r="F9" t="s">
         <v>3786</v>
@@ -14475,24 +14468,24 @@
         <v>42625</v>
       </c>
       <c r="H9" s="23">
-        <v>0.55585361111111109</v>
+        <v>0.55922932870370368</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>1709</v>
+        <v>553</v>
       </c>
       <c r="B10" t="s">
         <v>12</v>
       </c>
       <c r="C10">
-        <v>13</v>
+        <v>101</v>
       </c>
       <c r="D10">
-        <v>99</v>
+        <v>516</v>
       </c>
       <c r="E10" t="s">
-        <v>1710</v>
+        <v>554</v>
       </c>
       <c r="F10" t="s">
         <v>3786</v>
@@ -14501,24 +14494,24 @@
         <v>42625</v>
       </c>
       <c r="H10" s="23">
-        <v>0.55726989583333331</v>
+        <v>0.55922934027777782</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>1715</v>
+        <v>1654</v>
       </c>
       <c r="B11" t="s">
         <v>12</v>
       </c>
       <c r="C11">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D11">
-        <v>308</v>
+        <v>154</v>
       </c>
       <c r="E11" t="s">
-        <v>1716</v>
+        <v>1655</v>
       </c>
       <c r="F11" t="s">
         <v>3786</v>
@@ -14527,24 +14520,24 @@
         <v>42625</v>
       </c>
       <c r="H11" s="23">
-        <v>0.55726989583333331</v>
+        <v>0.55585361111111109</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>1731</v>
+        <v>1709</v>
       </c>
       <c r="B12" t="s">
         <v>12</v>
       </c>
       <c r="C12">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D12">
-        <v>60</v>
+        <v>99</v>
       </c>
       <c r="E12" t="s">
-        <v>1732</v>
+        <v>1710</v>
       </c>
       <c r="F12" t="s">
         <v>3786</v>
@@ -14553,24 +14546,24 @@
         <v>42625</v>
       </c>
       <c r="H12" s="23">
-        <v>0.55726994212962966</v>
+        <v>0.55726989583333331</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>1749</v>
+        <v>1715</v>
       </c>
       <c r="B13" t="s">
         <v>12</v>
       </c>
       <c r="C13">
-        <v>165</v>
+        <v>35</v>
       </c>
       <c r="D13">
-        <v>795</v>
+        <v>308</v>
       </c>
       <c r="E13" t="s">
-        <v>1750</v>
+        <v>1716</v>
       </c>
       <c r="F13" t="s">
         <v>3786</v>
@@ -14579,24 +14572,24 @@
         <v>42625</v>
       </c>
       <c r="H13" s="23">
-        <v>0.55922890046296303</v>
+        <v>0.55726989583333331</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>1774</v>
+        <v>1731</v>
       </c>
       <c r="B14" t="s">
         <v>12</v>
       </c>
       <c r="C14">
-        <v>165</v>
+        <v>11</v>
       </c>
       <c r="D14">
-        <v>755</v>
+        <v>60</v>
       </c>
       <c r="E14" t="s">
-        <v>1775</v>
+        <v>1732</v>
       </c>
       <c r="F14" t="s">
         <v>3786</v>
@@ -14605,24 +14598,24 @@
         <v>42625</v>
       </c>
       <c r="H14" s="23">
-        <v>0.55922876157407408</v>
+        <v>0.55726994212962966</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>1798</v>
+        <v>1749</v>
       </c>
       <c r="B15" t="s">
         <v>12</v>
       </c>
       <c r="C15">
-        <v>22</v>
+        <v>165</v>
       </c>
       <c r="D15">
-        <v>286</v>
+        <v>795</v>
       </c>
       <c r="E15" t="s">
-        <v>1799</v>
+        <v>1750</v>
       </c>
       <c r="F15" t="s">
         <v>3786</v>
@@ -14631,24 +14624,24 @@
         <v>42625</v>
       </c>
       <c r="H15" s="23">
-        <v>0.55922875000000005</v>
+        <v>0.55922890046296303</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>1800</v>
+        <v>1774</v>
       </c>
       <c r="B16" t="s">
         <v>12</v>
       </c>
       <c r="C16">
-        <v>21</v>
+        <v>165</v>
       </c>
       <c r="D16">
-        <v>214</v>
+        <v>755</v>
       </c>
       <c r="E16" t="s">
-        <v>1802</v>
+        <v>1775</v>
       </c>
       <c r="F16" t="s">
         <v>3786</v>
@@ -14657,24 +14650,24 @@
         <v>42625</v>
       </c>
       <c r="H16" s="23">
-        <v>0.55922891203703706</v>
+        <v>0.55922876157407408</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>2414</v>
+        <v>1798</v>
       </c>
       <c r="B17" t="s">
         <v>12</v>
       </c>
       <c r="C17">
-        <v>96</v>
+        <v>22</v>
       </c>
       <c r="D17">
-        <v>497</v>
+        <v>286</v>
       </c>
       <c r="E17" t="s">
-        <v>2415</v>
+        <v>1799</v>
       </c>
       <c r="F17" t="s">
         <v>3786</v>
@@ -14683,24 +14676,24 @@
         <v>42625</v>
       </c>
       <c r="H17" s="23">
-        <v>0.55709123842592589</v>
+        <v>0.55922875000000005</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>2416</v>
+        <v>1800</v>
       </c>
       <c r="B18" t="s">
         <v>12</v>
       </c>
       <c r="C18">
-        <v>60</v>
+        <v>21</v>
       </c>
       <c r="D18">
-        <v>329</v>
+        <v>214</v>
       </c>
       <c r="E18" t="s">
-        <v>2417</v>
+        <v>1802</v>
       </c>
       <c r="F18" t="s">
         <v>3786</v>
@@ -14709,255 +14702,249 @@
         <v>42625</v>
       </c>
       <c r="H18" s="23">
-        <v>0.55922960648148146</v>
+        <v>0.55922891203703706</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>3760</v>
+        <v>3644</v>
       </c>
       <c r="B19" t="s">
-        <v>3784</v>
+        <v>12</v>
       </c>
       <c r="C19">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="D19">
-        <v>708</v>
-      </c>
-      <c r="E19" t="s">
-        <v>3785</v>
+        <v>193</v>
       </c>
       <c r="F19" t="s">
         <v>3786</v>
       </c>
       <c r="G19" s="20">
-        <v>42867</v>
+        <v>40515</v>
       </c>
       <c r="H19" s="23">
-        <v>0.63624543981481485</v>
+        <v>0.37460487268518516</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>3761</v>
+        <v>2414</v>
       </c>
       <c r="B20" t="s">
-        <v>3784</v>
+        <v>12</v>
       </c>
       <c r="C20">
-        <v>9</v>
+        <v>96</v>
       </c>
       <c r="D20">
-        <v>445</v>
+        <v>497</v>
       </c>
       <c r="E20" t="s">
-        <v>3787</v>
+        <v>2415</v>
       </c>
       <c r="F20" t="s">
         <v>3786</v>
       </c>
       <c r="G20" s="20">
-        <v>42867</v>
+        <v>42625</v>
       </c>
       <c r="H20" s="23">
-        <v>0.63624543981481485</v>
+        <v>0.55709123842592589</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>3762</v>
+        <v>2416</v>
       </c>
       <c r="B21" t="s">
-        <v>3784</v>
+        <v>12</v>
       </c>
       <c r="C21">
-        <v>12</v>
+        <v>60</v>
       </c>
       <c r="D21">
-        <v>464</v>
+        <v>329</v>
       </c>
       <c r="E21" t="s">
-        <v>3788</v>
+        <v>2417</v>
       </c>
       <c r="F21" t="s">
         <v>3786</v>
       </c>
       <c r="G21" s="20">
-        <v>42650</v>
+        <v>42625</v>
       </c>
       <c r="H21" s="23">
-        <v>0.62406721064814819</v>
+        <v>0.55922960648148146</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>2448</v>
+        <v>3645</v>
       </c>
       <c r="B22" t="s">
         <v>12</v>
       </c>
       <c r="C22">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="D22">
-        <v>115</v>
-      </c>
-      <c r="E22" t="s">
-        <v>2449</v>
+        <v>637</v>
       </c>
       <c r="F22" t="s">
         <v>3786</v>
       </c>
       <c r="G22" s="20">
-        <v>42625</v>
+        <v>39486</v>
       </c>
       <c r="H22" s="23">
-        <v>0.55726989583333331</v>
+        <v>0.21075917824074075</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>2473</v>
+        <v>3760</v>
       </c>
       <c r="B23" t="s">
-        <v>12</v>
+        <v>3784</v>
       </c>
       <c r="C23">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="D23">
-        <v>243</v>
+        <v>708</v>
       </c>
       <c r="E23" t="s">
-        <v>2474</v>
+        <v>3785</v>
       </c>
       <c r="F23" t="s">
         <v>3786</v>
       </c>
       <c r="G23" s="20">
-        <v>42625</v>
+        <v>42867</v>
       </c>
       <c r="H23" s="23">
-        <v>0.55922956018518521</v>
+        <v>0.63624543981481485</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>2492</v>
+        <v>3761</v>
       </c>
       <c r="B24" t="s">
-        <v>12</v>
+        <v>3784</v>
       </c>
       <c r="C24">
-        <v>300</v>
+        <v>9</v>
       </c>
       <c r="D24">
-        <v>1757</v>
+        <v>445</v>
       </c>
       <c r="E24" t="s">
-        <v>2493</v>
+        <v>3787</v>
       </c>
       <c r="F24" t="s">
         <v>3786</v>
       </c>
       <c r="G24" s="20">
-        <v>42625</v>
+        <v>42867</v>
       </c>
       <c r="H24" s="23">
-        <v>0.55922916666666667</v>
+        <v>0.63624543981481485</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>2618</v>
+        <v>3762</v>
       </c>
       <c r="B25" t="s">
-        <v>12</v>
+        <v>3784</v>
       </c>
       <c r="C25">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="D25">
-        <v>173</v>
+        <v>464</v>
       </c>
       <c r="E25" t="s">
-        <v>2619</v>
+        <v>3788</v>
       </c>
       <c r="F25" t="s">
         <v>3786</v>
       </c>
       <c r="G25" s="20">
-        <v>42625</v>
+        <v>42650</v>
       </c>
       <c r="H25" s="23">
-        <v>0.55922890046296303</v>
+        <v>0.62406721064814819</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>2642</v>
+        <v>3763</v>
       </c>
       <c r="B26" t="s">
         <v>12</v>
       </c>
       <c r="C26">
-        <v>39</v>
+        <v>18</v>
       </c>
       <c r="D26">
-        <v>362</v>
+        <v>98</v>
       </c>
       <c r="E26" t="s">
-        <v>2643</v>
+        <v>3789</v>
       </c>
       <c r="F26" t="s">
         <v>3786</v>
       </c>
       <c r="G26" s="20">
-        <v>42625</v>
+        <v>42108</v>
       </c>
       <c r="H26" s="23">
-        <v>0.55922959490740742</v>
+        <v>0.64862504629629625</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>2667</v>
+        <v>3764</v>
       </c>
       <c r="B27" t="s">
         <v>12</v>
       </c>
       <c r="C27">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="D27">
-        <v>187</v>
-      </c>
-      <c r="E27" t="s">
-        <v>2668</v>
+        <v>114</v>
       </c>
       <c r="F27" t="s">
         <v>3786</v>
       </c>
       <c r="G27" s="20">
-        <v>42625</v>
+        <v>41006</v>
       </c>
       <c r="H27" s="23">
-        <v>0.55922890046296303</v>
+        <v>0.15572981481481482</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>2702</v>
+        <v>2448</v>
       </c>
       <c r="B28" t="s">
         <v>12</v>
       </c>
       <c r="C28">
-        <v>231</v>
+        <v>18</v>
       </c>
       <c r="D28">
-        <v>3720</v>
+        <v>115</v>
+      </c>
+      <c r="E28" t="s">
+        <v>2449</v>
       </c>
       <c r="F28" t="s">
         <v>3786</v>
@@ -14966,76 +14953,73 @@
         <v>42625</v>
       </c>
       <c r="H28" s="23">
-        <v>0.55922961805555549</v>
+        <v>0.55726989583333331</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>2721</v>
+        <v>2473</v>
       </c>
       <c r="B29" t="s">
         <v>12</v>
       </c>
       <c r="C29">
-        <v>84</v>
+        <v>40</v>
       </c>
       <c r="D29">
-        <v>691</v>
+        <v>243</v>
       </c>
       <c r="E29" t="s">
-        <v>2722</v>
+        <v>2474</v>
       </c>
       <c r="F29" t="s">
         <v>3786</v>
       </c>
       <c r="G29" s="20">
-        <v>42628</v>
+        <v>42625</v>
       </c>
       <c r="H29" s="23">
-        <v>0.59570064814814816</v>
+        <v>0.55922956018518521</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>2725</v>
+        <v>3765</v>
       </c>
       <c r="B30" t="s">
         <v>12</v>
       </c>
       <c r="C30">
-        <v>51</v>
+        <v>8</v>
       </c>
       <c r="D30">
-        <v>374</v>
-      </c>
-      <c r="E30" t="s">
-        <v>2726</v>
+        <v>52</v>
       </c>
       <c r="F30" t="s">
         <v>3786</v>
       </c>
       <c r="G30" s="20">
-        <v>42625</v>
+        <v>39478</v>
       </c>
       <c r="H30" s="23">
-        <v>0.55756822916666671</v>
+        <v>0.6515180439814815</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>2727</v>
+        <v>2492</v>
       </c>
       <c r="B31" t="s">
         <v>12</v>
       </c>
       <c r="C31">
-        <v>42</v>
+        <v>300</v>
       </c>
       <c r="D31">
-        <v>267</v>
+        <v>1757</v>
       </c>
       <c r="E31" t="s">
-        <v>2728</v>
+        <v>2493</v>
       </c>
       <c r="F31" t="s">
         <v>3786</v>
@@ -15044,539 +15028,545 @@
         <v>42625</v>
       </c>
       <c r="H31" s="23">
-        <v>0.55756824074074074</v>
+        <v>0.55922916666666667</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>2729</v>
+        <v>3766</v>
       </c>
       <c r="B32" t="s">
         <v>12</v>
       </c>
       <c r="C32">
-        <v>12</v>
+        <v>41</v>
       </c>
       <c r="D32">
-        <v>101</v>
-      </c>
-      <c r="E32" t="s">
-        <v>2730</v>
+        <v>276</v>
       </c>
       <c r="F32" t="s">
         <v>3786</v>
       </c>
       <c r="G32" s="20">
-        <v>42625</v>
+        <v>39487</v>
       </c>
       <c r="H32" s="23">
-        <v>0.55756821759259256</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+        <v>0.25032361111111112</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>3763</v>
+        <v>3767</v>
       </c>
       <c r="B33" t="s">
         <v>12</v>
       </c>
       <c r="C33">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="D33">
-        <v>98</v>
-      </c>
-      <c r="E33" t="s">
-        <v>3789</v>
+        <v>293</v>
       </c>
       <c r="F33" t="s">
         <v>3786</v>
       </c>
       <c r="G33" s="20">
-        <v>42108</v>
+        <v>39486</v>
       </c>
       <c r="H33" s="23">
-        <v>0.64862504629629625</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+        <v>0.29502784722222225</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>3769</v>
+        <v>3768</v>
       </c>
       <c r="B34" t="s">
         <v>12</v>
       </c>
       <c r="C34">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="D34">
-        <v>238</v>
-      </c>
-      <c r="E34" t="s">
-        <v>3790</v>
+        <v>92</v>
       </c>
       <c r="F34" t="s">
         <v>3786</v>
       </c>
       <c r="G34" s="20">
-        <v>41939</v>
+        <v>39486</v>
       </c>
       <c r="H34" s="23">
-        <v>0.86599032407407417</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+        <v>0.2950538425925926</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>3778</v>
+        <v>2618</v>
       </c>
       <c r="B35" t="s">
         <v>12</v>
       </c>
       <c r="C35">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="D35">
-        <v>115</v>
+        <v>173</v>
       </c>
       <c r="E35" t="s">
-        <v>3791</v>
+        <v>2619</v>
       </c>
       <c r="F35" t="s">
         <v>3786</v>
       </c>
       <c r="G35" s="20">
-        <v>41740</v>
+        <v>42625</v>
       </c>
       <c r="H35" s="23">
-        <v>0.62420861111111114</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+        <v>0.55922890046296303</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>3776</v>
+        <v>3769</v>
       </c>
       <c r="B36" t="s">
         <v>12</v>
       </c>
       <c r="C36">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D36">
-        <v>119</v>
+        <v>238</v>
+      </c>
+      <c r="E36" t="s">
+        <v>3790</v>
       </c>
       <c r="F36" t="s">
         <v>3786</v>
       </c>
       <c r="G36" s="20">
-        <v>41413</v>
+        <v>41939</v>
       </c>
       <c r="H36" s="23">
-        <v>8.7360601851851849E-2</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+        <v>0.86599032407407417</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>3777</v>
+        <v>3770</v>
       </c>
       <c r="B37" t="s">
         <v>12</v>
       </c>
       <c r="C37">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="D37">
-        <v>90</v>
+        <v>118</v>
       </c>
       <c r="F37" t="s">
         <v>3786</v>
       </c>
       <c r="G37" s="20">
-        <v>41413</v>
+        <v>41017</v>
       </c>
       <c r="H37" s="23">
-        <v>8.7362951388888888E-2</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+        <v>4.7388194444444439E-3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>3779</v>
+        <v>3771</v>
       </c>
       <c r="B38" t="s">
         <v>12</v>
       </c>
       <c r="C38">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="D38">
-        <v>411</v>
+        <v>135</v>
       </c>
       <c r="F38" t="s">
         <v>3786</v>
       </c>
       <c r="G38" s="20">
-        <v>41410</v>
+        <v>39370</v>
       </c>
       <c r="H38" s="23">
-        <v>0.50206951388888887</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+        <v>0.49657274305555554</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>3770</v>
+        <v>2642</v>
       </c>
       <c r="B39" t="s">
         <v>12</v>
       </c>
       <c r="C39">
-        <v>17</v>
+        <v>39</v>
       </c>
       <c r="D39">
-        <v>118</v>
+        <v>362</v>
+      </c>
+      <c r="E39" t="s">
+        <v>2643</v>
       </c>
       <c r="F39" t="s">
         <v>3786</v>
       </c>
       <c r="G39" s="20">
-        <v>41017</v>
+        <v>42625</v>
       </c>
       <c r="H39" s="23">
-        <v>4.7388194444444439E-3</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+        <v>0.55922959490740742</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>3764</v>
+        <v>3772</v>
       </c>
       <c r="B40" t="s">
         <v>12</v>
       </c>
       <c r="C40">
-        <v>19</v>
+        <v>37</v>
       </c>
       <c r="D40">
-        <v>114</v>
+        <v>282</v>
       </c>
       <c r="F40" t="s">
         <v>3786</v>
       </c>
       <c r="G40" s="20">
-        <v>41006</v>
+        <v>39303</v>
       </c>
       <c r="H40" s="23">
-        <v>0.15572981481481482</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+        <v>0.74039734953703695</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>3644</v>
+        <v>2667</v>
       </c>
       <c r="B41" t="s">
         <v>12</v>
       </c>
       <c r="C41">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D41">
-        <v>193</v>
+        <v>187</v>
+      </c>
+      <c r="E41" t="s">
+        <v>2668</v>
       </c>
       <c r="F41" t="s">
         <v>3786</v>
       </c>
       <c r="G41" s="20">
-        <v>40515</v>
+        <v>42625</v>
       </c>
       <c r="H41" s="23">
-        <v>0.37460487268518516</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+        <v>0.55922890046296303</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>3766</v>
+        <v>2702</v>
       </c>
       <c r="B42" t="s">
         <v>12</v>
       </c>
       <c r="C42">
-        <v>41</v>
+        <v>231</v>
       </c>
       <c r="D42">
-        <v>276</v>
+        <v>3720</v>
       </c>
       <c r="F42" t="s">
         <v>3786</v>
       </c>
       <c r="G42" s="20">
-        <v>39487</v>
+        <v>42625</v>
       </c>
       <c r="H42" s="23">
-        <v>0.25032361111111112</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+        <v>0.55922961805555549</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>3781</v>
+        <v>3773</v>
       </c>
       <c r="B43" t="s">
         <v>12</v>
       </c>
       <c r="C43">
-        <v>12</v>
+        <v>37</v>
       </c>
       <c r="D43">
-        <v>110</v>
+        <v>333</v>
       </c>
       <c r="F43" t="s">
         <v>3786</v>
       </c>
       <c r="G43" s="20">
-        <v>39486</v>
+        <v>39465</v>
       </c>
       <c r="H43" s="23">
-        <v>0.39357087962962961</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+        <v>0.51796172453703704</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>3645</v>
+        <v>2721</v>
       </c>
       <c r="B44" t="s">
         <v>12</v>
       </c>
       <c r="C44">
-        <v>9</v>
+        <v>84</v>
       </c>
       <c r="D44">
-        <v>637</v>
+        <v>691</v>
+      </c>
+      <c r="E44" t="s">
+        <v>2722</v>
       </c>
       <c r="F44" t="s">
         <v>3786</v>
       </c>
       <c r="G44" s="20">
-        <v>39486</v>
+        <v>42628</v>
       </c>
       <c r="H44" s="23">
-        <v>0.21075917824074075</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+        <v>0.59570064814814816</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>3767</v>
+        <v>2725</v>
       </c>
       <c r="B45" t="s">
         <v>12</v>
       </c>
       <c r="C45">
-        <v>30</v>
+        <v>51</v>
       </c>
       <c r="D45">
-        <v>293</v>
+        <v>374</v>
+      </c>
+      <c r="E45" t="s">
+        <v>2726</v>
       </c>
       <c r="F45" t="s">
         <v>3786</v>
       </c>
       <c r="G45" s="20">
-        <v>39486</v>
+        <v>42625</v>
       </c>
       <c r="H45" s="23">
-        <v>0.29502784722222225</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+        <v>0.55756822916666671</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>3768</v>
+        <v>2727</v>
       </c>
       <c r="B46" t="s">
         <v>12</v>
       </c>
       <c r="C46">
-        <v>14</v>
+        <v>42</v>
       </c>
       <c r="D46">
-        <v>92</v>
+        <v>267</v>
+      </c>
+      <c r="E46" t="s">
+        <v>2728</v>
       </c>
       <c r="F46" t="s">
         <v>3786</v>
       </c>
       <c r="G46" s="20">
-        <v>39486</v>
+        <v>42625</v>
       </c>
       <c r="H46" s="23">
-        <v>0.2950538425925926</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+        <v>0.55756824074074074</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>3765</v>
+        <v>3774</v>
       </c>
       <c r="B47" t="s">
         <v>12</v>
       </c>
       <c r="C47">
-        <v>8</v>
+        <v>92</v>
       </c>
       <c r="D47">
-        <v>52</v>
+        <v>675</v>
       </c>
       <c r="F47" t="s">
         <v>3786</v>
       </c>
       <c r="G47" s="20">
-        <v>39478</v>
+        <v>39072</v>
       </c>
       <c r="H47" s="23">
-        <v>0.6515180439814815</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+        <v>0.45860575231481482</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>3773</v>
+        <v>3775</v>
       </c>
       <c r="B48" t="s">
         <v>12</v>
       </c>
       <c r="C48">
-        <v>37</v>
+        <v>53</v>
       </c>
       <c r="D48">
-        <v>333</v>
+        <v>355</v>
       </c>
       <c r="F48" t="s">
         <v>3786</v>
       </c>
       <c r="G48" s="20">
-        <v>39465</v>
+        <v>39072</v>
       </c>
       <c r="H48" s="23">
-        <v>0.51796172453703704</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+        <v>0.45864018518518518</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>3771</v>
+        <v>3776</v>
       </c>
       <c r="B49" t="s">
         <v>12</v>
       </c>
       <c r="C49">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="D49">
-        <v>135</v>
+        <v>119</v>
       </c>
       <c r="F49" t="s">
         <v>3786</v>
       </c>
       <c r="G49" s="20">
-        <v>39370</v>
+        <v>41413</v>
       </c>
       <c r="H49" s="23">
-        <v>0.49657274305555554</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+        <v>8.7360601851851849E-2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>3772</v>
+        <v>3777</v>
       </c>
       <c r="B50" t="s">
         <v>12</v>
       </c>
       <c r="C50">
-        <v>37</v>
+        <v>12</v>
       </c>
       <c r="D50">
-        <v>282</v>
+        <v>90</v>
       </c>
       <c r="F50" t="s">
         <v>3786</v>
       </c>
       <c r="G50" s="20">
-        <v>39303</v>
+        <v>41413</v>
       </c>
       <c r="H50" s="23">
-        <v>0.74039734953703695</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+        <v>8.7362951388888888E-2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>3759</v>
+        <v>3778</v>
       </c>
       <c r="B51" t="s">
         <v>12</v>
       </c>
       <c r="C51">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="D51">
-        <v>87</v>
+        <v>115</v>
+      </c>
+      <c r="E51" t="s">
+        <v>3791</v>
       </c>
       <c r="F51" t="s">
         <v>3786</v>
       </c>
       <c r="G51" s="20">
-        <v>39121</v>
+        <v>41740</v>
       </c>
       <c r="H51" s="23">
-        <v>0.42892013888888886</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+        <v>0.62420861111111114</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>3774</v>
+        <v>2729</v>
       </c>
       <c r="B52" t="s">
         <v>12</v>
       </c>
       <c r="C52">
-        <v>92</v>
+        <v>12</v>
       </c>
       <c r="D52">
-        <v>675</v>
+        <v>101</v>
+      </c>
+      <c r="E52" t="s">
+        <v>2730</v>
       </c>
       <c r="F52" t="s">
         <v>3786</v>
       </c>
       <c r="G52" s="20">
-        <v>39072</v>
+        <v>42625</v>
       </c>
       <c r="H52" s="23">
-        <v>0.45860575231481482</v>
-      </c>
-    </row>
-    <row r="53" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+        <v>0.55756821759259256</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>3775</v>
+        <v>3779</v>
       </c>
       <c r="B53" t="s">
         <v>12</v>
       </c>
       <c r="C53">
-        <v>53</v>
+        <v>25</v>
       </c>
       <c r="D53">
-        <v>355</v>
+        <v>411</v>
       </c>
       <c r="F53" t="s">
         <v>3786</v>
       </c>
       <c r="G53" s="20">
-        <v>39072</v>
+        <v>41410</v>
       </c>
       <c r="H53" s="23">
-        <v>0.45864018518518518</v>
-      </c>
-    </row>
-    <row r="54" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="55" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="56" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
+        <v>0.50206951388888887</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:H56">
-    <filterColumn colId="6">
-      <filters>
-        <dateGroupItem year="2017" dateTimeGrouping="year"/>
-        <dateGroupItem year="2016" dateTimeGrouping="year"/>
-      </filters>
-    </filterColumn>
-    <sortState ref="A2:H32">
+    <sortState ref="A2:H56">
       <sortCondition ref="A1:A56"/>
     </sortState>
   </autoFilter>
@@ -15591,9 +15581,9 @@
   </sheetPr>
   <dimension ref="A1:L1996"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A611" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B630" sqref="B630"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="95.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -37908,7 +37898,7 @@
       </c>
     </row>
     <row r="631" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A631" t="s">
+      <c r="A631" s="22" t="s">
         <v>1137</v>
       </c>
       <c r="B631" t="s">
@@ -37980,7 +37970,7 @@
       </c>
     </row>
     <row r="633" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A633" t="s">
+      <c r="A633" s="22" t="s">
         <v>1135</v>
       </c>
       <c r="B633" t="s">

</xml_diff>